<commit_message>
hover returns point info, about to add popup
</commit_message>
<xml_diff>
--- a/data/DL_matrices_ID_WY.xlsx
+++ b/data/DL_matrices_ID_WY.xlsx
@@ -315,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -345,8 +345,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -357,20 +368,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BF42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:BE21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BF27" sqref="BF27:BF42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,301 +666,301 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:58" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="32"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="32"/>
-      <c r="AD3" s="32"/>
-      <c r="AE3" s="32"/>
-      <c r="AF3" s="32"/>
-      <c r="AG3" s="32"/>
-      <c r="AH3" s="32"/>
-      <c r="AI3" s="32"/>
-      <c r="AJ3" s="32"/>
-      <c r="AK3" s="32"/>
-      <c r="AL3" s="32"/>
-      <c r="AM3" s="32"/>
-      <c r="AN3" s="32"/>
-      <c r="AO3" s="32"/>
-      <c r="AP3" s="32"/>
-      <c r="AQ3" s="32"/>
-      <c r="AR3" s="32"/>
-      <c r="AS3" s="32"/>
-      <c r="AT3" s="32"/>
-      <c r="AU3" s="32"/>
-      <c r="AV3" s="32"/>
-      <c r="AW3" s="32"/>
-      <c r="AX3" s="32"/>
-      <c r="AY3" s="32"/>
-      <c r="AZ3" s="32"/>
-      <c r="BA3" s="32"/>
-      <c r="BB3" s="32"/>
-      <c r="BC3" s="32"/>
-      <c r="BD3" s="32"/>
-      <c r="BE3" s="32"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="35"/>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="35"/>
+      <c r="AK3" s="35"/>
+      <c r="AL3" s="35"/>
+      <c r="AM3" s="35"/>
+      <c r="AN3" s="35"/>
+      <c r="AO3" s="35"/>
+      <c r="AP3" s="35"/>
+      <c r="AQ3" s="35"/>
+      <c r="AR3" s="35"/>
+      <c r="AS3" s="35"/>
+      <c r="AT3" s="35"/>
+      <c r="AU3" s="35"/>
+      <c r="AV3" s="35"/>
+      <c r="AW3" s="35"/>
+      <c r="AX3" s="35"/>
+      <c r="AY3" s="35"/>
+      <c r="AZ3" s="35"/>
+      <c r="BA3" s="35"/>
+      <c r="BB3" s="35"/>
+      <c r="BC3" s="35"/>
+      <c r="BD3" s="35"/>
+      <c r="BE3" s="35"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="28"/>
-      <c r="AJ4" s="28"/>
-      <c r="AK4" s="28"/>
-      <c r="AL4" s="28"/>
-      <c r="AM4" s="28"/>
-      <c r="AN4" s="28"/>
-      <c r="AO4" s="28"/>
-      <c r="AP4" s="28"/>
-      <c r="AQ4" s="28"/>
-      <c r="AR4" s="28"/>
-      <c r="AS4" s="28"/>
-      <c r="AT4" s="28"/>
-      <c r="AU4" s="28"/>
-      <c r="AV4" s="28"/>
-      <c r="AW4" s="28"/>
-      <c r="AX4" s="28"/>
-      <c r="AY4" s="28"/>
-      <c r="AZ4" s="28"/>
-      <c r="BA4" s="28"/>
-      <c r="BB4" s="28"/>
-      <c r="BC4" s="28"/>
-      <c r="BD4" s="28"/>
-      <c r="BE4" s="28"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37"/>
+      <c r="AN4" s="37"/>
+      <c r="AO4" s="37"/>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="37"/>
+      <c r="AR4" s="37"/>
+      <c r="AS4" s="37"/>
+      <c r="AT4" s="37"/>
+      <c r="AU4" s="37"/>
+      <c r="AV4" s="37"/>
+      <c r="AW4" s="37"/>
+      <c r="AX4" s="37"/>
+      <c r="AY4" s="37"/>
+      <c r="AZ4" s="37"/>
+      <c r="BA4" s="37"/>
+      <c r="BB4" s="37"/>
+      <c r="BC4" s="37"/>
+      <c r="BD4" s="37"/>
+      <c r="BE4" s="37"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="34">
+      <c r="B5" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="28">
         <v>41</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="28">
         <v>42</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="28">
         <v>43</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="28">
         <v>44</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="28">
         <v>45</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="28">
         <v>46</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="28">
         <v>47</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="28">
         <v>48</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="28">
         <v>49</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="28">
         <v>50</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="28">
         <v>51</v>
       </c>
-      <c r="N5" s="34">
+      <c r="N5" s="28">
         <v>52</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="28">
         <v>53</v>
       </c>
-      <c r="P5" s="34">
+      <c r="P5" s="28">
         <v>54</v>
       </c>
-      <c r="Q5" s="34">
+      <c r="Q5" s="28">
         <v>55</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="28">
         <v>56</v>
       </c>
-      <c r="S5" s="34">
+      <c r="S5" s="28">
         <v>57</v>
       </c>
-      <c r="T5" s="34">
+      <c r="T5" s="28">
         <v>58</v>
       </c>
-      <c r="U5" s="34">
+      <c r="U5" s="28">
         <v>59</v>
       </c>
-      <c r="V5" s="34">
+      <c r="V5" s="28">
         <v>60</v>
       </c>
-      <c r="W5" s="34">
+      <c r="W5" s="28">
         <v>61</v>
       </c>
-      <c r="X5" s="34">
+      <c r="X5" s="28">
         <v>62</v>
       </c>
-      <c r="Y5" s="34">
+      <c r="Y5" s="28">
         <v>63</v>
       </c>
-      <c r="Z5" s="34">
+      <c r="Z5" s="28">
         <v>64</v>
       </c>
-      <c r="AA5" s="34">
+      <c r="AA5" s="28">
         <v>65</v>
       </c>
-      <c r="AB5" s="34">
+      <c r="AB5" s="28">
         <v>66</v>
       </c>
-      <c r="AC5" s="34">
+      <c r="AC5" s="28">
         <v>67</v>
       </c>
-      <c r="AD5" s="34">
+      <c r="AD5" s="28">
         <v>68</v>
       </c>
-      <c r="AE5" s="34">
+      <c r="AE5" s="28">
         <v>69</v>
       </c>
-      <c r="AF5" s="34">
+      <c r="AF5" s="28">
         <v>70</v>
       </c>
-      <c r="AG5" s="34">
+      <c r="AG5" s="28">
         <v>71</v>
       </c>
-      <c r="AH5" s="34">
+      <c r="AH5" s="28">
         <v>72</v>
       </c>
-      <c r="AI5" s="34">
+      <c r="AI5" s="28">
         <v>73</v>
       </c>
-      <c r="AJ5" s="34">
+      <c r="AJ5" s="28">
         <v>74</v>
       </c>
-      <c r="AK5" s="34">
+      <c r="AK5" s="28">
         <v>75</v>
       </c>
-      <c r="AL5" s="34">
+      <c r="AL5" s="28">
         <v>76</v>
       </c>
-      <c r="AM5" s="34">
+      <c r="AM5" s="28">
         <v>77</v>
       </c>
-      <c r="AN5" s="34">
+      <c r="AN5" s="28">
         <v>78</v>
       </c>
-      <c r="AO5" s="34">
+      <c r="AO5" s="28">
         <v>79</v>
       </c>
-      <c r="AP5" s="34">
+      <c r="AP5" s="28">
         <v>80</v>
       </c>
-      <c r="AQ5" s="34">
+      <c r="AQ5" s="28">
         <v>81</v>
       </c>
-      <c r="AR5" s="34">
+      <c r="AR5" s="28">
         <v>82</v>
       </c>
-      <c r="AS5" s="34">
+      <c r="AS5" s="28">
         <v>83</v>
       </c>
-      <c r="AT5" s="34">
+      <c r="AT5" s="28">
         <v>84</v>
       </c>
-      <c r="AU5" s="34">
+      <c r="AU5" s="28">
         <v>85</v>
       </c>
-      <c r="AV5" s="34">
+      <c r="AV5" s="28">
         <v>86</v>
       </c>
-      <c r="AW5" s="34">
+      <c r="AW5" s="28">
         <v>87</v>
       </c>
-      <c r="AX5" s="34">
+      <c r="AX5" s="28">
         <v>88</v>
       </c>
-      <c r="AY5" s="34">
+      <c r="AY5" s="28">
         <v>89</v>
       </c>
-      <c r="AZ5" s="34">
+      <c r="AZ5" s="28">
         <v>90</v>
       </c>
-      <c r="BA5" s="34">
+      <c r="BA5" s="28">
         <v>91</v>
       </c>
-      <c r="BB5" s="34">
+      <c r="BB5" s="28">
         <v>92</v>
       </c>
-      <c r="BC5" s="34">
+      <c r="BC5" s="28">
         <v>93</v>
       </c>
-      <c r="BD5" s="34">
+      <c r="BD5" s="28">
         <v>94</v>
       </c>
-      <c r="BE5" s="35" t="s">
+      <c r="BE5" s="29" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="36">
+      <c r="A6" s="36"/>
+      <c r="B6" s="30">
         <v>4</v>
       </c>
       <c r="C6" s="4"/>
@@ -1028,16 +1025,16 @@
       <c r="BB6" s="2"/>
       <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
-      <c r="BE6" s="37">
+      <c r="BE6" s="31">
         <v>5</v>
       </c>
-      <c r="BF6" s="31" t="s">
+      <c r="BF6" s="36" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="36">
+      <c r="A7" s="36"/>
+      <c r="B7" s="30">
         <v>5</v>
       </c>
       <c r="C7" s="4"/>
@@ -1138,14 +1135,14 @@
         <v>1</v>
       </c>
       <c r="BD7" s="2"/>
-      <c r="BE7" s="37">
+      <c r="BE7" s="31">
         <v>53</v>
       </c>
-      <c r="BF7" s="31"/>
+      <c r="BF7" s="36"/>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="36">
+      <c r="A8" s="36"/>
+      <c r="B8" s="30">
         <v>6</v>
       </c>
       <c r="C8" s="4"/>
@@ -1258,14 +1255,14 @@
       <c r="BB8" s="2"/>
       <c r="BC8" s="2"/>
       <c r="BD8" s="2"/>
-      <c r="BE8" s="37">
+      <c r="BE8" s="31">
         <v>102</v>
       </c>
-      <c r="BF8" s="31"/>
+      <c r="BF8" s="36"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="36">
+      <c r="A9" s="36"/>
+      <c r="B9" s="30">
         <v>7</v>
       </c>
       <c r="C9" s="4"/>
@@ -1384,14 +1381,14 @@
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
-      <c r="BE9" s="37">
+      <c r="BE9" s="31">
         <v>73</v>
       </c>
-      <c r="BF9" s="31"/>
+      <c r="BF9" s="36"/>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="36">
+      <c r="A10" s="36"/>
+      <c r="B10" s="30">
         <v>8</v>
       </c>
       <c r="C10" s="4"/>
@@ -1496,14 +1493,14 @@
       <c r="BB10" s="3"/>
       <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
-      <c r="BE10" s="37">
+      <c r="BE10" s="31">
         <v>55</v>
       </c>
-      <c r="BF10" s="31"/>
+      <c r="BF10" s="36"/>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="36">
+      <c r="A11" s="36"/>
+      <c r="B11" s="30">
         <v>9</v>
       </c>
       <c r="C11" s="4"/>
@@ -1604,14 +1601,14 @@
       <c r="BB11" s="3"/>
       <c r="BC11" s="3"/>
       <c r="BD11" s="3"/>
-      <c r="BE11" s="37">
+      <c r="BE11" s="31">
         <v>42</v>
       </c>
-      <c r="BF11" s="31"/>
+      <c r="BF11" s="36"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="36">
+      <c r="A12" s="36"/>
+      <c r="B12" s="30">
         <v>10</v>
       </c>
       <c r="C12" s="4"/>
@@ -1696,14 +1693,14 @@
       <c r="BB12" s="3"/>
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
-      <c r="BE12" s="37">
+      <c r="BE12" s="31">
         <v>24</v>
       </c>
-      <c r="BF12" s="31"/>
+      <c r="BF12" s="36"/>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="36">
+      <c r="A13" s="36"/>
+      <c r="B13" s="30">
         <v>11</v>
       </c>
       <c r="C13" s="4"/>
@@ -1782,14 +1779,14 @@
       <c r="BB13" s="4"/>
       <c r="BC13" s="4"/>
       <c r="BD13" s="4"/>
-      <c r="BE13" s="37">
+      <c r="BE13" s="31">
         <v>13</v>
       </c>
-      <c r="BF13" s="31"/>
+      <c r="BF13" s="36"/>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="36">
+      <c r="A14" s="36"/>
+      <c r="B14" s="30">
         <v>12</v>
       </c>
       <c r="C14" s="4"/>
@@ -1864,14 +1861,14 @@
       <c r="BB14" s="4"/>
       <c r="BC14" s="4"/>
       <c r="BD14" s="4"/>
-      <c r="BE14" s="37">
+      <c r="BE14" s="31">
         <v>10</v>
       </c>
-      <c r="BF14" s="31"/>
+      <c r="BF14" s="36"/>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="36">
+      <c r="A15" s="36"/>
+      <c r="B15" s="30">
         <v>13</v>
       </c>
       <c r="C15" s="4"/>
@@ -1944,14 +1941,14 @@
       <c r="BB15" s="4"/>
       <c r="BC15" s="4"/>
       <c r="BD15" s="4"/>
-      <c r="BE15" s="37">
+      <c r="BE15" s="31">
         <v>8</v>
       </c>
-      <c r="BF15" s="31"/>
+      <c r="BF15" s="36"/>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="36">
+      <c r="A16" s="36"/>
+      <c r="B16" s="30">
         <v>14</v>
       </c>
       <c r="C16" s="4"/>
@@ -2018,14 +2015,14 @@
       <c r="BB16" s="4"/>
       <c r="BC16" s="4"/>
       <c r="BD16" s="4"/>
-      <c r="BE16" s="37">
+      <c r="BE16" s="31">
         <v>7</v>
       </c>
-      <c r="BF16" s="31"/>
+      <c r="BF16" s="36"/>
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="36">
+      <c r="A17" s="36"/>
+      <c r="B17" s="30">
         <v>15</v>
       </c>
       <c r="C17" s="4"/>
@@ -2086,14 +2083,14 @@
       <c r="BB17" s="4"/>
       <c r="BC17" s="4"/>
       <c r="BD17" s="4"/>
-      <c r="BE17" s="37">
-        <v>2</v>
-      </c>
-      <c r="BF17" s="31"/>
+      <c r="BE17" s="31">
+        <v>2</v>
+      </c>
+      <c r="BF17" s="36"/>
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="36">
+      <c r="A18" s="36"/>
+      <c r="B18" s="30">
         <v>16</v>
       </c>
       <c r="C18" s="4"/>
@@ -2152,14 +2149,14 @@
       <c r="BB18" s="4"/>
       <c r="BC18" s="4"/>
       <c r="BD18" s="4"/>
-      <c r="BE18" s="37">
-        <v>1</v>
-      </c>
-      <c r="BF18" s="31"/>
+      <c r="BE18" s="31">
+        <v>1</v>
+      </c>
+      <c r="BF18" s="36"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="36">
+      <c r="A19" s="36"/>
+      <c r="B19" s="30">
         <v>17</v>
       </c>
       <c r="C19" s="4"/>
@@ -2218,14 +2215,14 @@
       <c r="BB19" s="4"/>
       <c r="BC19" s="4"/>
       <c r="BD19" s="4"/>
-      <c r="BE19" s="37">
-        <v>1</v>
-      </c>
-      <c r="BF19" s="31"/>
+      <c r="BE19" s="31">
+        <v>1</v>
+      </c>
+      <c r="BF19" s="36"/>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="36">
+      <c r="A20" s="36"/>
+      <c r="B20" s="30">
         <v>18</v>
       </c>
       <c r="C20" s="4"/>
@@ -2282,182 +2279,182 @@
       <c r="BB20" s="4"/>
       <c r="BC20" s="4"/>
       <c r="BD20" s="4"/>
-      <c r="BE20" s="37">
-        <v>0</v>
-      </c>
-      <c r="BF20" s="31"/>
+      <c r="BE20" s="31">
+        <v>0</v>
+      </c>
+      <c r="BF20" s="36"/>
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="39">
-        <v>0</v>
-      </c>
-      <c r="D21" s="39">
-        <v>1</v>
-      </c>
-      <c r="E21" s="39">
-        <v>2</v>
-      </c>
-      <c r="F21" s="39">
-        <v>1</v>
-      </c>
-      <c r="G21" s="39">
+      <c r="A21" s="36"/>
+      <c r="B21" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <v>1</v>
+      </c>
+      <c r="E21" s="33">
+        <v>2</v>
+      </c>
+      <c r="F21" s="33">
+        <v>1</v>
+      </c>
+      <c r="G21" s="33">
         <v>5</v>
       </c>
-      <c r="H21" s="39">
-        <v>2</v>
-      </c>
-      <c r="I21" s="39">
+      <c r="H21" s="33">
+        <v>2</v>
+      </c>
+      <c r="I21" s="33">
         <v>5</v>
       </c>
-      <c r="J21" s="39">
-        <v>2</v>
-      </c>
-      <c r="K21" s="39">
+      <c r="J21" s="33">
+        <v>2</v>
+      </c>
+      <c r="K21" s="33">
         <v>4</v>
       </c>
-      <c r="L21" s="39">
-        <v>1</v>
-      </c>
-      <c r="M21" s="39">
+      <c r="L21" s="33">
+        <v>1</v>
+      </c>
+      <c r="M21" s="33">
         <v>5</v>
       </c>
-      <c r="N21" s="39">
-        <v>2</v>
-      </c>
-      <c r="O21" s="39">
+      <c r="N21" s="33">
+        <v>2</v>
+      </c>
+      <c r="O21" s="33">
         <v>6</v>
       </c>
-      <c r="P21" s="39">
+      <c r="P21" s="33">
         <v>7</v>
       </c>
-      <c r="Q21" s="39">
-        <v>2</v>
-      </c>
-      <c r="R21" s="39">
+      <c r="Q21" s="33">
+        <v>2</v>
+      </c>
+      <c r="R21" s="33">
         <v>3</v>
       </c>
-      <c r="S21" s="39">
+      <c r="S21" s="33">
         <v>10</v>
       </c>
-      <c r="T21" s="39">
+      <c r="T21" s="33">
         <v>8</v>
       </c>
-      <c r="U21" s="39">
+      <c r="U21" s="33">
         <v>5</v>
       </c>
-      <c r="V21" s="39">
+      <c r="V21" s="33">
         <v>14</v>
       </c>
-      <c r="W21" s="39">
+      <c r="W21" s="33">
         <v>6</v>
       </c>
-      <c r="X21" s="39">
+      <c r="X21" s="33">
         <v>8</v>
       </c>
-      <c r="Y21" s="39">
+      <c r="Y21" s="33">
         <v>7</v>
       </c>
-      <c r="Z21" s="39">
+      <c r="Z21" s="33">
         <v>8</v>
       </c>
-      <c r="AA21" s="39">
+      <c r="AA21" s="33">
         <v>5</v>
       </c>
-      <c r="AB21" s="39">
+      <c r="AB21" s="33">
         <v>10</v>
       </c>
-      <c r="AC21" s="39">
+      <c r="AC21" s="33">
         <v>6</v>
       </c>
-      <c r="AD21" s="39">
+      <c r="AD21" s="33">
         <v>7</v>
       </c>
-      <c r="AE21" s="39">
+      <c r="AE21" s="33">
         <v>9</v>
       </c>
-      <c r="AF21" s="39">
+      <c r="AF21" s="33">
         <v>12</v>
       </c>
-      <c r="AG21" s="39">
+      <c r="AG21" s="33">
         <v>17</v>
       </c>
-      <c r="AH21" s="39">
+      <c r="AH21" s="33">
         <v>20</v>
       </c>
-      <c r="AI21" s="39">
+      <c r="AI21" s="33">
         <v>14</v>
       </c>
-      <c r="AJ21" s="39">
+      <c r="AJ21" s="33">
         <v>19</v>
       </c>
-      <c r="AK21" s="39">
+      <c r="AK21" s="33">
         <v>15</v>
       </c>
-      <c r="AL21" s="39">
+      <c r="AL21" s="33">
         <v>16</v>
       </c>
-      <c r="AM21" s="39">
+      <c r="AM21" s="33">
         <v>13</v>
       </c>
-      <c r="AN21" s="39">
+      <c r="AN21" s="33">
         <v>13</v>
       </c>
-      <c r="AO21" s="39">
+      <c r="AO21" s="33">
         <v>8</v>
       </c>
-      <c r="AP21" s="39">
+      <c r="AP21" s="33">
         <v>15</v>
       </c>
-      <c r="AQ21" s="39">
+      <c r="AQ21" s="33">
         <v>15</v>
       </c>
-      <c r="AR21" s="39">
+      <c r="AR21" s="33">
         <v>12</v>
       </c>
-      <c r="AS21" s="39">
+      <c r="AS21" s="33">
         <v>11</v>
       </c>
-      <c r="AT21" s="39">
+      <c r="AT21" s="33">
         <v>12</v>
       </c>
-      <c r="AU21" s="39">
+      <c r="AU21" s="33">
         <v>7</v>
       </c>
-      <c r="AV21" s="39">
+      <c r="AV21" s="33">
         <v>4</v>
       </c>
-      <c r="AW21" s="39">
+      <c r="AW21" s="33">
         <v>7</v>
       </c>
-      <c r="AX21" s="39">
+      <c r="AX21" s="33">
         <v>5</v>
       </c>
-      <c r="AY21" s="39">
+      <c r="AY21" s="33">
         <v>4</v>
       </c>
-      <c r="AZ21" s="39">
-        <v>2</v>
-      </c>
-      <c r="BA21" s="39">
-        <v>2</v>
-      </c>
-      <c r="BB21" s="39">
-        <v>1</v>
-      </c>
-      <c r="BC21" s="39">
-        <v>1</v>
-      </c>
-      <c r="BD21" s="39">
-        <v>0</v>
-      </c>
-      <c r="BE21" s="40">
+      <c r="AZ21" s="33">
+        <v>2</v>
+      </c>
+      <c r="BA21" s="33">
+        <v>2</v>
+      </c>
+      <c r="BB21" s="33">
+        <v>1</v>
+      </c>
+      <c r="BC21" s="33">
+        <v>1</v>
+      </c>
+      <c r="BD21" s="33">
+        <v>0</v>
+      </c>
+      <c r="BE21" s="34">
         <v>396</v>
       </c>
-      <c r="BF21" s="31"/>
+      <c r="BF21" s="36"/>
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" s="26"/>
@@ -2577,128 +2574,128 @@
       <c r="BD23" s="1"/>
       <c r="BE23" s="1"/>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="B24" s="27" t="s">
+    <row r="24" spans="1:58" ht="18" x14ac:dyDescent="0.35">
+      <c r="B24" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="27"/>
-      <c r="AC24" s="27"/>
-      <c r="AD24" s="27"/>
-      <c r="AE24" s="27"/>
-      <c r="AF24" s="27"/>
-      <c r="AG24" s="27"/>
-      <c r="AH24" s="27"/>
-      <c r="AI24" s="27"/>
-      <c r="AJ24" s="27"/>
-      <c r="AK24" s="27"/>
-      <c r="AL24" s="27"/>
-      <c r="AM24" s="27"/>
-      <c r="AN24" s="27"/>
-      <c r="AO24" s="27"/>
-      <c r="AP24" s="27"/>
-      <c r="AQ24" s="27"/>
-      <c r="AR24" s="27"/>
-      <c r="AS24" s="27"/>
-      <c r="AT24" s="27"/>
-      <c r="AU24" s="27"/>
-      <c r="AV24" s="27"/>
-      <c r="AW24" s="27"/>
-      <c r="AX24" s="27"/>
-      <c r="AY24" s="27"/>
-      <c r="AZ24" s="27"/>
-      <c r="BA24" s="27"/>
-      <c r="BB24" s="27"/>
-      <c r="BC24" s="27"/>
-      <c r="BD24" s="27"/>
-      <c r="BE24" s="27"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="35"/>
+      <c r="Z24" s="35"/>
+      <c r="AA24" s="35"/>
+      <c r="AB24" s="35"/>
+      <c r="AC24" s="35"/>
+      <c r="AD24" s="35"/>
+      <c r="AE24" s="35"/>
+      <c r="AF24" s="35"/>
+      <c r="AG24" s="35"/>
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="35"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
+      <c r="AL24" s="35"/>
+      <c r="AM24" s="35"/>
+      <c r="AN24" s="35"/>
+      <c r="AO24" s="35"/>
+      <c r="AP24" s="35"/>
+      <c r="AQ24" s="35"/>
+      <c r="AR24" s="35"/>
+      <c r="AS24" s="35"/>
+      <c r="AT24" s="35"/>
+      <c r="AU24" s="35"/>
+      <c r="AV24" s="35"/>
+      <c r="AW24" s="35"/>
+      <c r="AX24" s="35"/>
+      <c r="AY24" s="35"/>
+      <c r="AZ24" s="35"/>
+      <c r="BA24" s="35"/>
+      <c r="BB24" s="35"/>
+      <c r="BC24" s="35"/>
+      <c r="BD24" s="35"/>
+      <c r="BE24" s="35"/>
     </row>
     <row r="25" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="28"/>
-      <c r="AH25" s="28"/>
-      <c r="AI25" s="28"/>
-      <c r="AJ25" s="28"/>
-      <c r="AK25" s="28"/>
-      <c r="AL25" s="28"/>
-      <c r="AM25" s="28"/>
-      <c r="AN25" s="28"/>
-      <c r="AO25" s="28"/>
-      <c r="AP25" s="28"/>
-      <c r="AQ25" s="28"/>
-      <c r="AR25" s="28"/>
-      <c r="AS25" s="28"/>
-      <c r="AT25" s="28"/>
-      <c r="AU25" s="28"/>
-      <c r="AV25" s="28"/>
-      <c r="AW25" s="28"/>
-      <c r="AX25" s="28"/>
-      <c r="AY25" s="28"/>
-      <c r="AZ25" s="28"/>
-      <c r="BA25" s="28"/>
-      <c r="BB25" s="28"/>
-      <c r="BC25" s="28"/>
-      <c r="BD25" s="28"/>
-      <c r="BE25" s="28"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="37"/>
+      <c r="Z25" s="37"/>
+      <c r="AA25" s="37"/>
+      <c r="AB25" s="37"/>
+      <c r="AC25" s="37"/>
+      <c r="AD25" s="37"/>
+      <c r="AE25" s="37"/>
+      <c r="AF25" s="37"/>
+      <c r="AG25" s="37"/>
+      <c r="AH25" s="37"/>
+      <c r="AI25" s="37"/>
+      <c r="AJ25" s="37"/>
+      <c r="AK25" s="37"/>
+      <c r="AL25" s="37"/>
+      <c r="AM25" s="37"/>
+      <c r="AN25" s="37"/>
+      <c r="AO25" s="37"/>
+      <c r="AP25" s="37"/>
+      <c r="AQ25" s="37"/>
+      <c r="AR25" s="37"/>
+      <c r="AS25" s="37"/>
+      <c r="AT25" s="37"/>
+      <c r="AU25" s="37"/>
+      <c r="AV25" s="37"/>
+      <c r="AW25" s="37"/>
+      <c r="AX25" s="37"/>
+      <c r="AY25" s="37"/>
+      <c r="AZ25" s="37"/>
+      <c r="BA25" s="37"/>
+      <c r="BB25" s="37"/>
+      <c r="BC25" s="37"/>
+      <c r="BD25" s="37"/>
+      <c r="BE25" s="37"/>
     </row>
     <row r="26" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2871,7 +2868,7 @@
       </c>
     </row>
     <row r="27" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="1">
         <v>4</v>
       </c>
@@ -2936,12 +2933,12 @@
       <c r="BE27" s="1">
         <v>2</v>
       </c>
-      <c r="BF27" s="31" t="s">
+      <c r="BF27" s="36" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="1">
         <v>5</v>
       </c>
@@ -3018,10 +3015,10 @@
       <c r="BE28" s="1">
         <v>15</v>
       </c>
-      <c r="BF28" s="31"/>
+      <c r="BF28" s="36"/>
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A29" s="31"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="1">
         <v>6</v>
       </c>
@@ -3100,10 +3097,10 @@
       <c r="BE29" s="1">
         <v>11</v>
       </c>
-      <c r="BF29" s="31"/>
+      <c r="BF29" s="36"/>
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="1">
         <v>7</v>
       </c>
@@ -3176,10 +3173,10 @@
       <c r="BE30" s="1">
         <v>8</v>
       </c>
-      <c r="BF30" s="31"/>
+      <c r="BF30" s="36"/>
     </row>
     <row r="31" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="1">
         <v>8</v>
       </c>
@@ -3250,10 +3247,10 @@
       <c r="BE31" s="1">
         <v>6</v>
       </c>
-      <c r="BF31" s="31"/>
+      <c r="BF31" s="36"/>
     </row>
     <row r="32" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="1">
         <v>9</v>
       </c>
@@ -3326,10 +3323,10 @@
       <c r="BE32" s="1">
         <v>7</v>
       </c>
-      <c r="BF32" s="31"/>
+      <c r="BF32" s="36"/>
     </row>
     <row r="33" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A33" s="31"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="1">
         <v>10</v>
       </c>
@@ -3392,10 +3389,10 @@
       <c r="BE33" s="1">
         <v>1</v>
       </c>
-      <c r="BF33" s="31"/>
+      <c r="BF33" s="36"/>
     </row>
     <row r="34" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A34" s="31"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="1">
         <v>11</v>
       </c>
@@ -3456,10 +3453,10 @@
       <c r="BE34" s="1">
         <v>0</v>
       </c>
-      <c r="BF34" s="31"/>
+      <c r="BF34" s="36"/>
     </row>
     <row r="35" spans="1:58" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="1">
         <v>12</v>
       </c>
@@ -3520,12 +3517,12 @@
       <c r="BE35" s="1">
         <v>0</v>
       </c>
-      <c r="BF35" s="31" t="s">
+      <c r="BF35" s="36" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A36" s="31"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="1">
         <v>13</v>
       </c>
@@ -3586,10 +3583,10 @@
       <c r="BE36" s="1">
         <v>0</v>
       </c>
-      <c r="BF36" s="31"/>
+      <c r="BF36" s="36"/>
     </row>
     <row r="37" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A37" s="31"/>
+      <c r="A37" s="36"/>
       <c r="B37" s="1">
         <v>14</v>
       </c>
@@ -3650,10 +3647,10 @@
       <c r="BE37" s="1">
         <v>0</v>
       </c>
-      <c r="BF37" s="31"/>
+      <c r="BF37" s="36"/>
     </row>
     <row r="38" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A38" s="31"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="1">
         <v>15</v>
       </c>
@@ -3714,10 +3711,10 @@
       <c r="BE38" s="1">
         <v>0</v>
       </c>
-      <c r="BF38" s="31"/>
+      <c r="BF38" s="36"/>
     </row>
     <row r="39" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A39" s="31"/>
+      <c r="A39" s="36"/>
       <c r="B39" s="1">
         <v>16</v>
       </c>
@@ -3778,10 +3775,10 @@
       <c r="BE39" s="1">
         <v>0</v>
       </c>
-      <c r="BF39" s="31"/>
+      <c r="BF39" s="36"/>
     </row>
     <row r="40" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A40" s="31"/>
+      <c r="A40" s="36"/>
       <c r="B40" s="1">
         <v>17</v>
       </c>
@@ -3842,10 +3839,10 @@
       <c r="BE40" s="1">
         <v>0</v>
       </c>
-      <c r="BF40" s="31"/>
+      <c r="BF40" s="36"/>
     </row>
     <row r="41" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A41" s="31"/>
+      <c r="A41" s="36"/>
       <c r="B41" s="1">
         <v>18</v>
       </c>
@@ -3906,10 +3903,10 @@
       <c r="BE41" s="1">
         <v>0</v>
       </c>
-      <c r="BF41" s="31"/>
+      <c r="BF41" s="36"/>
     </row>
     <row r="42" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A42" s="31"/>
+      <c r="A42" s="36"/>
       <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
@@ -4078,7 +4075,7 @@
       <c r="BE42" s="1">
         <v>50</v>
       </c>
-      <c r="BF42" s="31"/>
+      <c r="BF42" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6190,122 +6187,122 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:58" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
-      <c r="AN2" s="30"/>
-      <c r="AO2" s="30"/>
-      <c r="AP2" s="30"/>
-      <c r="AQ2" s="30"/>
-      <c r="AR2" s="30"/>
-      <c r="AS2" s="30"/>
-      <c r="AT2" s="30"/>
-      <c r="AU2" s="30"/>
-      <c r="AV2" s="30"/>
-      <c r="AW2" s="30"/>
-      <c r="AX2" s="30"/>
-      <c r="AY2" s="30"/>
-      <c r="AZ2" s="30"/>
-      <c r="BA2" s="30"/>
-      <c r="BB2" s="30"/>
-      <c r="BC2" s="30"/>
-      <c r="BD2" s="30"/>
-      <c r="BE2" s="30"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
+      <c r="AN2" s="39"/>
+      <c r="AO2" s="39"/>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="39"/>
+      <c r="AR2" s="39"/>
+      <c r="AS2" s="39"/>
+      <c r="AT2" s="39"/>
+      <c r="AU2" s="39"/>
+      <c r="AV2" s="39"/>
+      <c r="AW2" s="39"/>
+      <c r="AX2" s="39"/>
+      <c r="AY2" s="39"/>
+      <c r="AZ2" s="39"/>
+      <c r="BA2" s="39"/>
+      <c r="BB2" s="39"/>
+      <c r="BC2" s="39"/>
+      <c r="BD2" s="39"/>
+      <c r="BE2" s="39"/>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="28"/>
-      <c r="AJ3" s="28"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="28"/>
-      <c r="AO3" s="28"/>
-      <c r="AP3" s="28"/>
-      <c r="AQ3" s="28"/>
-      <c r="AR3" s="28"/>
-      <c r="AS3" s="28"/>
-      <c r="AT3" s="28"/>
-      <c r="AU3" s="28"/>
-      <c r="AV3" s="28"/>
-      <c r="AW3" s="28"/>
-      <c r="AX3" s="28"/>
-      <c r="AY3" s="28"/>
-      <c r="AZ3" s="28"/>
-      <c r="BA3" s="28"/>
-      <c r="BB3" s="28"/>
-      <c r="BC3" s="28"/>
-      <c r="BD3" s="28"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AO3" s="37"/>
+      <c r="AP3" s="37"/>
+      <c r="AQ3" s="37"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="37"/>
+      <c r="AT3" s="37"/>
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
+      <c r="AW3" s="37"/>
+      <c r="AX3" s="37"/>
+      <c r="AY3" s="37"/>
+      <c r="AZ3" s="37"/>
+      <c r="BA3" s="37"/>
+      <c r="BB3" s="37"/>
+      <c r="BC3" s="37"/>
+      <c r="BD3" s="37"/>
     </row>
     <row r="4" spans="1:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -6478,7 +6475,7 @@
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B5">
@@ -6549,12 +6546,12 @@
       <c r="BE5">
         <v>7</v>
       </c>
-      <c r="BF5" s="29" t="s">
+      <c r="BF5" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
+      <c r="A6" s="38"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -6653,10 +6650,10 @@
       <c r="BE6">
         <v>59</v>
       </c>
-      <c r="BF6" s="29"/>
+      <c r="BF6" s="38"/>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+      <c r="A7" s="38"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -6765,10 +6762,10 @@
       <c r="BE7">
         <v>87</v>
       </c>
-      <c r="BF7" s="29"/>
+      <c r="BF7" s="38"/>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="38"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -6883,10 +6880,10 @@
       <c r="BE8">
         <v>51</v>
       </c>
-      <c r="BF8" s="29"/>
+      <c r="BF8" s="38"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
+      <c r="A9" s="38"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -6989,10 +6986,10 @@
       <c r="BE9">
         <v>45</v>
       </c>
-      <c r="BF9" s="29"/>
+      <c r="BF9" s="38"/>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
+      <c r="A10" s="38"/>
       <c r="B10">
         <v>9</v>
       </c>
@@ -7087,10 +7084,10 @@
       <c r="BE10">
         <v>31</v>
       </c>
-      <c r="BF10" s="29"/>
+      <c r="BF10" s="38"/>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
+      <c r="A11" s="38"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -7181,10 +7178,10 @@
       <c r="BE11">
         <v>27</v>
       </c>
-      <c r="BF11" s="29"/>
+      <c r="BF11" s="38"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
+      <c r="A12" s="38"/>
       <c r="B12">
         <v>11</v>
       </c>
@@ -7267,10 +7264,10 @@
       <c r="BE12">
         <v>13</v>
       </c>
-      <c r="BF12" s="29"/>
+      <c r="BF12" s="38"/>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
+      <c r="A13" s="38"/>
       <c r="B13">
         <v>12</v>
       </c>
@@ -7347,10 +7344,10 @@
       <c r="BE13">
         <v>9</v>
       </c>
-      <c r="BF13" s="29"/>
+      <c r="BF13" s="38"/>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="38"/>
       <c r="B14">
         <v>13</v>
       </c>
@@ -7417,10 +7414,10 @@
       <c r="BE14">
         <v>3</v>
       </c>
-      <c r="BF14" s="29"/>
+      <c r="BF14" s="38"/>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
+      <c r="A15" s="38"/>
       <c r="B15">
         <v>14</v>
       </c>
@@ -7489,10 +7486,10 @@
       <c r="BE15">
         <v>4</v>
       </c>
-      <c r="BF15" s="29"/>
+      <c r="BF15" s="38"/>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
+      <c r="A16" s="38"/>
       <c r="B16">
         <v>15</v>
       </c>
@@ -7555,10 +7552,10 @@
       <c r="BE16">
         <v>1</v>
       </c>
-      <c r="BF16" s="29"/>
+      <c r="BF16" s="38"/>
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A17" s="29"/>
+      <c r="A17" s="38"/>
       <c r="B17">
         <v>16</v>
       </c>
@@ -7621,10 +7618,10 @@
       <c r="BE17">
         <v>1</v>
       </c>
-      <c r="BF17" s="29"/>
+      <c r="BF17" s="38"/>
     </row>
     <row r="18" spans="1:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
+      <c r="A18" s="38"/>
       <c r="B18">
         <v>17</v>
       </c>
@@ -7685,7 +7682,7 @@
       <c r="BE18">
         <v>0</v>
       </c>
-      <c r="BF18" s="29"/>
+      <c r="BF18" s="38"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -7858,122 +7855,122 @@
       </c>
     </row>
     <row r="21" spans="1:58" ht="21" x14ac:dyDescent="0.4">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="30"/>
-      <c r="Z21" s="30"/>
-      <c r="AA21" s="30"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="30"/>
-      <c r="AD21" s="30"/>
-      <c r="AE21" s="30"/>
-      <c r="AF21" s="30"/>
-      <c r="AG21" s="30"/>
-      <c r="AH21" s="30"/>
-      <c r="AI21" s="30"/>
-      <c r="AJ21" s="30"/>
-      <c r="AK21" s="30"/>
-      <c r="AL21" s="30"/>
-      <c r="AM21" s="30"/>
-      <c r="AN21" s="30"/>
-      <c r="AO21" s="30"/>
-      <c r="AP21" s="30"/>
-      <c r="AQ21" s="30"/>
-      <c r="AR21" s="30"/>
-      <c r="AS21" s="30"/>
-      <c r="AT21" s="30"/>
-      <c r="AU21" s="30"/>
-      <c r="AV21" s="30"/>
-      <c r="AW21" s="30"/>
-      <c r="AX21" s="30"/>
-      <c r="AY21" s="30"/>
-      <c r="AZ21" s="30"/>
-      <c r="BA21" s="30"/>
-      <c r="BB21" s="30"/>
-      <c r="BC21" s="30"/>
-      <c r="BD21" s="30"/>
-      <c r="BE21" s="30"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="39"/>
+      <c r="Z21" s="39"/>
+      <c r="AA21" s="39"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="39"/>
+      <c r="AD21" s="39"/>
+      <c r="AE21" s="39"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="39"/>
+      <c r="AH21" s="39"/>
+      <c r="AI21" s="39"/>
+      <c r="AJ21" s="39"/>
+      <c r="AK21" s="39"/>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="39"/>
+      <c r="AO21" s="39"/>
+      <c r="AP21" s="39"/>
+      <c r="AQ21" s="39"/>
+      <c r="AR21" s="39"/>
+      <c r="AS21" s="39"/>
+      <c r="AT21" s="39"/>
+      <c r="AU21" s="39"/>
+      <c r="AV21" s="39"/>
+      <c r="AW21" s="39"/>
+      <c r="AX21" s="39"/>
+      <c r="AY21" s="39"/>
+      <c r="AZ21" s="39"/>
+      <c r="BA21" s="39"/>
+      <c r="BB21" s="39"/>
+      <c r="BC21" s="39"/>
+      <c r="BD21" s="39"/>
+      <c r="BE21" s="39"/>
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="28"/>
-      <c r="AH22" s="28"/>
-      <c r="AI22" s="28"/>
-      <c r="AJ22" s="28"/>
-      <c r="AK22" s="28"/>
-      <c r="AL22" s="28"/>
-      <c r="AM22" s="28"/>
-      <c r="AN22" s="28"/>
-      <c r="AO22" s="28"/>
-      <c r="AP22" s="28"/>
-      <c r="AQ22" s="28"/>
-      <c r="AR22" s="28"/>
-      <c r="AS22" s="28"/>
-      <c r="AT22" s="28"/>
-      <c r="AU22" s="28"/>
-      <c r="AV22" s="28"/>
-      <c r="AW22" s="28"/>
-      <c r="AX22" s="28"/>
-      <c r="AY22" s="28"/>
-      <c r="AZ22" s="28"/>
-      <c r="BA22" s="28"/>
-      <c r="BB22" s="28"/>
-      <c r="BC22" s="28"/>
-      <c r="BD22" s="28"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="37"/>
+      <c r="Z22" s="37"/>
+      <c r="AA22" s="37"/>
+      <c r="AB22" s="37"/>
+      <c r="AC22" s="37"/>
+      <c r="AD22" s="37"/>
+      <c r="AE22" s="37"/>
+      <c r="AF22" s="37"/>
+      <c r="AG22" s="37"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="37"/>
+      <c r="AJ22" s="37"/>
+      <c r="AK22" s="37"/>
+      <c r="AL22" s="37"/>
+      <c r="AM22" s="37"/>
+      <c r="AN22" s="37"/>
+      <c r="AO22" s="37"/>
+      <c r="AP22" s="37"/>
+      <c r="AQ22" s="37"/>
+      <c r="AR22" s="37"/>
+      <c r="AS22" s="37"/>
+      <c r="AT22" s="37"/>
+      <c r="AU22" s="37"/>
+      <c r="AV22" s="37"/>
+      <c r="AW22" s="37"/>
+      <c r="AX22" s="37"/>
+      <c r="AY22" s="37"/>
+      <c r="AZ22" s="37"/>
+      <c r="BA22" s="37"/>
+      <c r="BB22" s="37"/>
+      <c r="BC22" s="37"/>
+      <c r="BD22" s="37"/>
     </row>
     <row r="23" spans="1:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
@@ -8146,7 +8143,7 @@
       </c>
     </row>
     <row r="24" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B24">
@@ -8211,12 +8208,12 @@
       <c r="BE24">
         <v>3</v>
       </c>
-      <c r="BF24" s="29" t="s">
+      <c r="BF24" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
+      <c r="A25" s="38"/>
       <c r="B25">
         <v>5</v>
       </c>
@@ -8297,10 +8294,10 @@
       <c r="BE25">
         <v>20</v>
       </c>
-      <c r="BF25" s="29"/>
+      <c r="BF25" s="38"/>
     </row>
     <row r="26" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A26" s="29"/>
+      <c r="A26" s="38"/>
       <c r="B26">
         <v>6</v>
       </c>
@@ -8373,10 +8370,10 @@
       <c r="BE26">
         <v>17</v>
       </c>
-      <c r="BF26" s="29"/>
+      <c r="BF26" s="38"/>
     </row>
     <row r="27" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
+      <c r="A27" s="38"/>
       <c r="B27">
         <v>7</v>
       </c>
@@ -8447,10 +8444,10 @@
       <c r="BE27">
         <v>6</v>
       </c>
-      <c r="BF27" s="29"/>
+      <c r="BF27" s="38"/>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
+      <c r="A28" s="38"/>
       <c r="B28">
         <v>8</v>
       </c>
@@ -8517,10 +8514,10 @@
       <c r="BE28">
         <v>3</v>
       </c>
-      <c r="BF28" s="29"/>
+      <c r="BF28" s="38"/>
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
+      <c r="A29" s="38"/>
       <c r="B29">
         <v>9</v>
       </c>
@@ -8587,10 +8584,10 @@
       <c r="BE29">
         <v>3</v>
       </c>
-      <c r="BF29" s="29"/>
+      <c r="BF29" s="38"/>
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B30">
@@ -8657,10 +8654,10 @@
       <c r="BE30">
         <v>2</v>
       </c>
-      <c r="BF30" s="29"/>
+      <c r="BF30" s="38"/>
     </row>
     <row r="31" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A31" s="29"/>
+      <c r="A31" s="38"/>
       <c r="B31">
         <v>11</v>
       </c>
@@ -8723,12 +8720,12 @@
       <c r="BE31">
         <v>1</v>
       </c>
-      <c r="BF31" s="29" t="s">
+      <c r="BF31" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A32" s="29"/>
+      <c r="A32" s="38"/>
       <c r="B32">
         <v>12</v>
       </c>
@@ -8789,10 +8786,10 @@
       <c r="BE32">
         <v>0</v>
       </c>
-      <c r="BF32" s="29"/>
+      <c r="BF32" s="38"/>
     </row>
     <row r="33" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A33" s="29"/>
+      <c r="A33" s="38"/>
       <c r="B33">
         <v>13</v>
       </c>
@@ -8853,10 +8850,10 @@
       <c r="BE33">
         <v>0</v>
       </c>
-      <c r="BF33" s="29"/>
+      <c r="BF33" s="38"/>
     </row>
     <row r="34" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A34" s="29"/>
+      <c r="A34" s="38"/>
       <c r="B34">
         <v>14</v>
       </c>
@@ -8917,10 +8914,10 @@
       <c r="BE34">
         <v>0</v>
       </c>
-      <c r="BF34" s="29"/>
+      <c r="BF34" s="38"/>
     </row>
     <row r="35" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A35" s="29"/>
+      <c r="A35" s="38"/>
       <c r="B35">
         <v>15</v>
       </c>
@@ -8981,10 +8978,10 @@
       <c r="BE35">
         <v>0</v>
       </c>
-      <c r="BF35" s="29"/>
+      <c r="BF35" s="38"/>
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A36" s="29"/>
+      <c r="A36" s="38"/>
       <c r="B36">
         <v>16</v>
       </c>
@@ -9045,10 +9042,10 @@
       <c r="BE36">
         <v>0</v>
       </c>
-      <c r="BF36" s="29"/>
+      <c r="BF36" s="38"/>
     </row>
     <row r="37" spans="1:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="29"/>
+      <c r="A37" s="38"/>
       <c r="B37">
         <v>17</v>
       </c>
@@ -9109,7 +9106,7 @@
       <c r="BE37">
         <v>0</v>
       </c>
-      <c r="BF37" s="29"/>
+      <c r="BF37" s="38"/>
     </row>
     <row r="38" spans="1:58" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
@@ -9292,136 +9289,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="30"/>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="39"/>
+      <c r="AP1" s="39"/>
+      <c r="AQ1" s="39"/>
+      <c r="AR1" s="39"/>
+      <c r="AS1" s="39"/>
+      <c r="AT1" s="39"/>
+      <c r="AU1" s="39"/>
+      <c r="AV1" s="39"/>
+      <c r="AW1" s="39"/>
+      <c r="AX1" s="39"/>
+      <c r="AY1" s="39"/>
+      <c r="AZ1" s="39"/>
+      <c r="BA1" s="39"/>
+      <c r="BB1" s="39"/>
+      <c r="BC1" s="39"/>
+      <c r="BD1" s="39"/>
+      <c r="BE1" s="39"/>
+      <c r="BF1" s="39"/>
+      <c r="BG1" s="39"/>
+      <c r="BH1" s="39"/>
+      <c r="BI1" s="39"/>
+      <c r="BJ1" s="39"/>
+      <c r="BK1" s="39"/>
+      <c r="BL1" s="39"/>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
-      <c r="AQ2" s="28"/>
-      <c r="AR2" s="28"/>
-      <c r="AS2" s="28"/>
-      <c r="AT2" s="28"/>
-      <c r="AU2" s="28"/>
-      <c r="AV2" s="28"/>
-      <c r="AW2" s="28"/>
-      <c r="AX2" s="28"/>
-      <c r="AY2" s="28"/>
-      <c r="AZ2" s="28"/>
-      <c r="BA2" s="28"/>
-      <c r="BB2" s="28"/>
-      <c r="BC2" s="28"/>
-      <c r="BD2" s="28"/>
-      <c r="BE2" s="28"/>
-      <c r="BF2" s="28"/>
-      <c r="BG2" s="28"/>
-      <c r="BH2" s="28"/>
-      <c r="BI2" s="28"/>
-      <c r="BJ2" s="28"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="37"/>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="C3">
@@ -9609,7 +9606,7 @@
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -9684,12 +9681,12 @@
       <c r="BK4">
         <v>2</v>
       </c>
-      <c r="BL4" s="29" t="s">
+      <c r="BL4" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="38"/>
       <c r="B5">
         <v>4</v>
       </c>
@@ -9794,10 +9791,10 @@
       <c r="BK5">
         <v>40</v>
       </c>
-      <c r="BL5" s="29"/>
+      <c r="BL5" s="38"/>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
+      <c r="A6" s="38"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -9916,10 +9913,10 @@
       <c r="BK6">
         <v>175</v>
       </c>
-      <c r="BL6" s="29"/>
+      <c r="BL6" s="38"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+      <c r="A7" s="38"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -10054,10 +10051,10 @@
       <c r="BK7">
         <v>149</v>
       </c>
-      <c r="BL7" s="29"/>
+      <c r="BL7" s="38"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="38"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -10188,10 +10185,10 @@
       <c r="BK8">
         <v>82</v>
       </c>
-      <c r="BL8" s="29"/>
+      <c r="BL8" s="38"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
+      <c r="A9" s="38"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -10330,10 +10327,10 @@
       <c r="BK9">
         <v>59</v>
       </c>
-      <c r="BL9" s="29"/>
+      <c r="BL9" s="38"/>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
+      <c r="A10" s="38"/>
       <c r="B10">
         <v>9</v>
       </c>
@@ -10470,10 +10467,10 @@
       <c r="BK10">
         <v>35</v>
       </c>
-      <c r="BL10" s="29"/>
+      <c r="BL10" s="38"/>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
+      <c r="A11" s="38"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -10602,10 +10599,10 @@
       <c r="BK11">
         <v>36</v>
       </c>
-      <c r="BL11" s="29"/>
+      <c r="BL11" s="38"/>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
+      <c r="A12" s="38"/>
       <c r="B12">
         <v>11</v>
       </c>
@@ -10730,10 +10727,10 @@
       <c r="BK12">
         <v>14</v>
       </c>
-      <c r="BL12" s="29"/>
+      <c r="BL12" s="38"/>
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
+      <c r="A13" s="38"/>
       <c r="B13">
         <v>12</v>
       </c>
@@ -10842,10 +10839,10 @@
       <c r="BK13">
         <v>16</v>
       </c>
-      <c r="BL13" s="29"/>
+      <c r="BL13" s="38"/>
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="38"/>
       <c r="B14">
         <v>13</v>
       </c>
@@ -10932,10 +10929,10 @@
       <c r="BK14">
         <v>6</v>
       </c>
-      <c r="BL14" s="29"/>
+      <c r="BL14" s="38"/>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
+      <c r="A15" s="38"/>
       <c r="B15">
         <v>14</v>
       </c>
@@ -11018,10 +11015,10 @@
       <c r="BK15">
         <v>2</v>
       </c>
-      <c r="BL15" s="29"/>
+      <c r="BL15" s="38"/>
     </row>
     <row r="16" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
+      <c r="A16" s="38"/>
       <c r="B16">
         <v>15</v>
       </c>
@@ -11098,10 +11095,10 @@
       <c r="BK16">
         <v>3</v>
       </c>
-      <c r="BL16" s="29"/>
+      <c r="BL16" s="38"/>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A17" s="29"/>
+      <c r="A17" s="38"/>
       <c r="B17">
         <v>16</v>
       </c>
@@ -11176,10 +11173,10 @@
       <c r="BK17">
         <v>1</v>
       </c>
-      <c r="BL17" s="29"/>
+      <c r="BL17" s="38"/>
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
+      <c r="A18" s="38"/>
       <c r="B18">
         <v>17</v>
       </c>
@@ -11248,7 +11245,7 @@
       <c r="BK18">
         <v>0</v>
       </c>
-      <c r="BL18" s="29"/>
+      <c r="BL18" s="38"/>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -11439,136 +11436,136 @@
       </c>
     </row>
     <row r="21" spans="1:64" ht="21" x14ac:dyDescent="0.4">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="30"/>
-      <c r="Z21" s="30"/>
-      <c r="AA21" s="30"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="30"/>
-      <c r="AD21" s="30"/>
-      <c r="AE21" s="30"/>
-      <c r="AF21" s="30"/>
-      <c r="AG21" s="30"/>
-      <c r="AH21" s="30"/>
-      <c r="AI21" s="30"/>
-      <c r="AJ21" s="30"/>
-      <c r="AK21" s="30"/>
-      <c r="AL21" s="30"/>
-      <c r="AM21" s="30"/>
-      <c r="AN21" s="30"/>
-      <c r="AO21" s="30"/>
-      <c r="AP21" s="30"/>
-      <c r="AQ21" s="30"/>
-      <c r="AR21" s="30"/>
-      <c r="AS21" s="30"/>
-      <c r="AT21" s="30"/>
-      <c r="AU21" s="30"/>
-      <c r="AV21" s="30"/>
-      <c r="AW21" s="30"/>
-      <c r="AX21" s="30"/>
-      <c r="AY21" s="30"/>
-      <c r="AZ21" s="30"/>
-      <c r="BA21" s="30"/>
-      <c r="BB21" s="30"/>
-      <c r="BC21" s="30"/>
-      <c r="BD21" s="30"/>
-      <c r="BE21" s="30"/>
-      <c r="BF21" s="30"/>
-      <c r="BG21" s="30"/>
-      <c r="BH21" s="30"/>
-      <c r="BI21" s="30"/>
-      <c r="BJ21" s="30"/>
-      <c r="BK21" s="30"/>
-      <c r="BL21" s="30"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="39"/>
+      <c r="Z21" s="39"/>
+      <c r="AA21" s="39"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="39"/>
+      <c r="AD21" s="39"/>
+      <c r="AE21" s="39"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="39"/>
+      <c r="AH21" s="39"/>
+      <c r="AI21" s="39"/>
+      <c r="AJ21" s="39"/>
+      <c r="AK21" s="39"/>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="39"/>
+      <c r="AO21" s="39"/>
+      <c r="AP21" s="39"/>
+      <c r="AQ21" s="39"/>
+      <c r="AR21" s="39"/>
+      <c r="AS21" s="39"/>
+      <c r="AT21" s="39"/>
+      <c r="AU21" s="39"/>
+      <c r="AV21" s="39"/>
+      <c r="AW21" s="39"/>
+      <c r="AX21" s="39"/>
+      <c r="AY21" s="39"/>
+      <c r="AZ21" s="39"/>
+      <c r="BA21" s="39"/>
+      <c r="BB21" s="39"/>
+      <c r="BC21" s="39"/>
+      <c r="BD21" s="39"/>
+      <c r="BE21" s="39"/>
+      <c r="BF21" s="39"/>
+      <c r="BG21" s="39"/>
+      <c r="BH21" s="39"/>
+      <c r="BI21" s="39"/>
+      <c r="BJ21" s="39"/>
+      <c r="BK21" s="39"/>
+      <c r="BL21" s="39"/>
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="28"/>
-      <c r="AH22" s="28"/>
-      <c r="AI22" s="28"/>
-      <c r="AJ22" s="28"/>
-      <c r="AK22" s="28"/>
-      <c r="AL22" s="28"/>
-      <c r="AM22" s="28"/>
-      <c r="AN22" s="28"/>
-      <c r="AO22" s="28"/>
-      <c r="AP22" s="28"/>
-      <c r="AQ22" s="28"/>
-      <c r="AR22" s="28"/>
-      <c r="AS22" s="28"/>
-      <c r="AT22" s="28"/>
-      <c r="AU22" s="28"/>
-      <c r="AV22" s="28"/>
-      <c r="AW22" s="28"/>
-      <c r="AX22" s="28"/>
-      <c r="AY22" s="28"/>
-      <c r="AZ22" s="28"/>
-      <c r="BA22" s="28"/>
-      <c r="BB22" s="28"/>
-      <c r="BC22" s="28"/>
-      <c r="BD22" s="28"/>
-      <c r="BE22" s="28"/>
-      <c r="BF22" s="28"/>
-      <c r="BG22" s="28"/>
-      <c r="BH22" s="28"/>
-      <c r="BI22" s="28"/>
-      <c r="BJ22" s="28"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="37"/>
+      <c r="Z22" s="37"/>
+      <c r="AA22" s="37"/>
+      <c r="AB22" s="37"/>
+      <c r="AC22" s="37"/>
+      <c r="AD22" s="37"/>
+      <c r="AE22" s="37"/>
+      <c r="AF22" s="37"/>
+      <c r="AG22" s="37"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="37"/>
+      <c r="AJ22" s="37"/>
+      <c r="AK22" s="37"/>
+      <c r="AL22" s="37"/>
+      <c r="AM22" s="37"/>
+      <c r="AN22" s="37"/>
+      <c r="AO22" s="37"/>
+      <c r="AP22" s="37"/>
+      <c r="AQ22" s="37"/>
+      <c r="AR22" s="37"/>
+      <c r="AS22" s="37"/>
+      <c r="AT22" s="37"/>
+      <c r="AU22" s="37"/>
+      <c r="AV22" s="37"/>
+      <c r="AW22" s="37"/>
+      <c r="AX22" s="37"/>
+      <c r="AY22" s="37"/>
+      <c r="AZ22" s="37"/>
+      <c r="BA22" s="37"/>
+      <c r="BB22" s="37"/>
+      <c r="BC22" s="37"/>
+      <c r="BD22" s="37"/>
+      <c r="BE22" s="37"/>
+      <c r="BF22" s="37"/>
+      <c r="BG22" s="37"/>
+      <c r="BH22" s="37"/>
+      <c r="BI22" s="37"/>
+      <c r="BJ22" s="37"/>
     </row>
     <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="C23">
@@ -11756,7 +11753,7 @@
       </c>
     </row>
     <row r="24" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B24">
@@ -11825,12 +11822,12 @@
       <c r="BK24">
         <v>0</v>
       </c>
-      <c r="BL24" s="29" t="s">
+      <c r="BL24" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
+      <c r="A25" s="38"/>
       <c r="B25">
         <v>4</v>
       </c>
@@ -11903,10 +11900,10 @@
       <c r="BK25">
         <v>20</v>
       </c>
-      <c r="BL25" s="29"/>
+      <c r="BL25" s="38"/>
     </row>
     <row r="26" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A26" s="29"/>
+      <c r="A26" s="38"/>
       <c r="B26">
         <v>5</v>
       </c>
@@ -12001,10 +11998,10 @@
       <c r="BK26">
         <v>56</v>
       </c>
-      <c r="BL26" s="29"/>
+      <c r="BL26" s="38"/>
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
+      <c r="A27" s="38"/>
       <c r="B27">
         <v>6</v>
       </c>
@@ -12089,10 +12086,10 @@
       <c r="BK27">
         <v>17</v>
       </c>
-      <c r="BL27" s="29"/>
+      <c r="BL27" s="38"/>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
+      <c r="A28" s="38"/>
       <c r="B28">
         <v>7</v>
       </c>
@@ -12163,10 +12160,10 @@
       <c r="BK28">
         <v>3</v>
       </c>
-      <c r="BL28" s="29"/>
+      <c r="BL28" s="38"/>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
+      <c r="A29" s="38"/>
       <c r="B29">
         <v>8</v>
       </c>
@@ -12243,10 +12240,10 @@
       <c r="BK29">
         <v>11</v>
       </c>
-      <c r="BL29" s="29"/>
+      <c r="BL29" s="38"/>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A30" s="29"/>
+      <c r="A30" s="38"/>
       <c r="B30">
         <v>9</v>
       </c>
@@ -12315,10 +12312,10 @@
       <c r="BK30">
         <v>1</v>
       </c>
-      <c r="BL30" s="29"/>
+      <c r="BL30" s="38"/>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A31" s="29"/>
+      <c r="A31" s="38"/>
       <c r="B31">
         <v>10</v>
       </c>
@@ -12385,10 +12382,10 @@
       <c r="BK31">
         <v>0</v>
       </c>
-      <c r="BL31" s="29"/>
+      <c r="BL31" s="38"/>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A32" s="29"/>
+      <c r="A32" s="38"/>
       <c r="B32">
         <v>11</v>
       </c>
@@ -12457,10 +12454,10 @@
       <c r="BK32">
         <v>1</v>
       </c>
-      <c r="BL32" s="29"/>
+      <c r="BL32" s="38"/>
     </row>
     <row r="33" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A33" s="29"/>
+      <c r="A33" s="38"/>
       <c r="B33">
         <v>12</v>
       </c>
@@ -12527,10 +12524,10 @@
       <c r="BK33">
         <v>0</v>
       </c>
-      <c r="BL33" s="29"/>
+      <c r="BL33" s="38"/>
     </row>
     <row r="34" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A34" s="29"/>
+      <c r="A34" s="38"/>
       <c r="B34">
         <v>13</v>
       </c>
@@ -12597,10 +12594,10 @@
       <c r="BK34">
         <v>0</v>
       </c>
-      <c r="BL34" s="29"/>
+      <c r="BL34" s="38"/>
     </row>
     <row r="35" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A35" s="29"/>
+      <c r="A35" s="38"/>
       <c r="B35">
         <v>14</v>
       </c>
@@ -12667,10 +12664,10 @@
       <c r="BK35">
         <v>0</v>
       </c>
-      <c r="BL35" s="29"/>
+      <c r="BL35" s="38"/>
     </row>
     <row r="36" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A36" s="29"/>
+      <c r="A36" s="38"/>
       <c r="B36">
         <v>15</v>
       </c>
@@ -12737,10 +12734,10 @@
       <c r="BK36">
         <v>0</v>
       </c>
-      <c r="BL36" s="29"/>
+      <c r="BL36" s="38"/>
     </row>
     <row r="37" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A37" s="29"/>
+      <c r="A37" s="38"/>
       <c r="B37">
         <v>16</v>
       </c>
@@ -12807,10 +12804,10 @@
       <c r="BK37">
         <v>0</v>
       </c>
-      <c r="BL37" s="29"/>
+      <c r="BL37" s="38"/>
     </row>
     <row r="38" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A38" s="29"/>
+      <c r="A38" s="38"/>
       <c r="B38">
         <v>17</v>
       </c>
@@ -12877,7 +12874,7 @@
       <c r="BK38">
         <v>0</v>
       </c>
-      <c r="BL38" s="29"/>
+      <c r="BL38" s="38"/>
     </row>
     <row r="39" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
@@ -13101,135 +13098,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="30"/>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="39"/>
+      <c r="AP1" s="39"/>
+      <c r="AQ1" s="39"/>
+      <c r="AR1" s="39"/>
+      <c r="AS1" s="39"/>
+      <c r="AT1" s="39"/>
+      <c r="AU1" s="39"/>
+      <c r="AV1" s="39"/>
+      <c r="AW1" s="39"/>
+      <c r="AX1" s="39"/>
+      <c r="AY1" s="39"/>
+      <c r="AZ1" s="39"/>
+      <c r="BA1" s="39"/>
+      <c r="BB1" s="39"/>
+      <c r="BC1" s="39"/>
+      <c r="BD1" s="39"/>
+      <c r="BE1" s="39"/>
+      <c r="BF1" s="39"/>
+      <c r="BG1" s="39"/>
+      <c r="BH1" s="39"/>
+      <c r="BI1" s="39"/>
+      <c r="BJ1" s="39"/>
+      <c r="BK1" s="39"/>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
-      <c r="AQ2" s="28"/>
-      <c r="AR2" s="28"/>
-      <c r="AS2" s="28"/>
-      <c r="AT2" s="28"/>
-      <c r="AU2" s="28"/>
-      <c r="AV2" s="28"/>
-      <c r="AW2" s="28"/>
-      <c r="AX2" s="28"/>
-      <c r="AY2" s="28"/>
-      <c r="AZ2" s="28"/>
-      <c r="BA2" s="28"/>
-      <c r="BB2" s="28"/>
-      <c r="BC2" s="28"/>
-      <c r="BD2" s="28"/>
-      <c r="BE2" s="28"/>
-      <c r="BF2" s="28"/>
-      <c r="BG2" s="28"/>
-      <c r="BH2" s="28"/>
-      <c r="BI2" s="28"/>
-      <c r="BJ2" s="28"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="37"/>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -13420,7 +13417,7 @@
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -13495,12 +13492,12 @@
       <c r="BK4">
         <v>2</v>
       </c>
-      <c r="BL4" s="29" t="s">
+      <c r="BL4" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="38"/>
       <c r="B5">
         <v>4</v>
       </c>
@@ -13605,10 +13602,10 @@
       <c r="BK5">
         <v>36</v>
       </c>
-      <c r="BL5" s="29"/>
+      <c r="BL5" s="38"/>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
+      <c r="A6" s="38"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -13727,10 +13724,10 @@
       <c r="BK6">
         <v>131</v>
       </c>
-      <c r="BL6" s="29"/>
+      <c r="BL6" s="38"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+      <c r="A7" s="38"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -13865,10 +13862,10 @@
       <c r="BK7">
         <v>112</v>
       </c>
-      <c r="BL7" s="29"/>
+      <c r="BL7" s="38"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="38"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -13999,10 +13996,10 @@
       <c r="BK8">
         <v>60</v>
       </c>
-      <c r="BL8" s="29"/>
+      <c r="BL8" s="38"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
+      <c r="A9" s="38"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -14141,10 +14138,10 @@
       <c r="BK9">
         <v>50</v>
       </c>
-      <c r="BL9" s="29"/>
+      <c r="BL9" s="38"/>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
+      <c r="A10" s="38"/>
       <c r="B10">
         <v>9</v>
       </c>
@@ -14281,10 +14278,10 @@
       <c r="BK10">
         <v>31</v>
       </c>
-      <c r="BL10" s="29"/>
+      <c r="BL10" s="38"/>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
+      <c r="A11" s="38"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -14413,10 +14410,10 @@
       <c r="BK11">
         <v>22</v>
       </c>
-      <c r="BL11" s="29"/>
+      <c r="BL11" s="38"/>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
+      <c r="A12" s="38"/>
       <c r="B12">
         <v>11</v>
       </c>
@@ -14541,10 +14538,10 @@
       <c r="BK12">
         <v>20</v>
       </c>
-      <c r="BL12" s="29"/>
+      <c r="BL12" s="38"/>
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
+      <c r="A13" s="38"/>
       <c r="B13">
         <v>12</v>
       </c>
@@ -14653,10 +14650,10 @@
       <c r="BK13">
         <v>15</v>
       </c>
-      <c r="BL13" s="29"/>
+      <c r="BL13" s="38"/>
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="38"/>
       <c r="B14">
         <v>13</v>
       </c>
@@ -14743,10 +14740,10 @@
       <c r="BK14">
         <v>6</v>
       </c>
-      <c r="BL14" s="29"/>
+      <c r="BL14" s="38"/>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
+      <c r="A15" s="38"/>
       <c r="B15">
         <v>14</v>
       </c>
@@ -14829,10 +14826,10 @@
       <c r="BK15">
         <v>9</v>
       </c>
-      <c r="BL15" s="29"/>
+      <c r="BL15" s="38"/>
     </row>
     <row r="16" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
+      <c r="A16" s="38"/>
       <c r="B16">
         <v>15</v>
       </c>
@@ -14909,10 +14906,10 @@
       <c r="BK16">
         <v>2</v>
       </c>
-      <c r="BL16" s="29"/>
+      <c r="BL16" s="38"/>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A17" s="29"/>
+      <c r="A17" s="38"/>
       <c r="B17">
         <v>16</v>
       </c>
@@ -14987,10 +14984,10 @@
       <c r="BK17">
         <v>0</v>
       </c>
-      <c r="BL17" s="29"/>
+      <c r="BL17" s="38"/>
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
+      <c r="A18" s="38"/>
       <c r="B18">
         <v>17</v>
       </c>
@@ -15059,7 +15056,7 @@
       <c r="BK18">
         <v>0</v>
       </c>
-      <c r="BL18" s="29"/>
+      <c r="BL18" s="38"/>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -15250,135 +15247,135 @@
       </c>
     </row>
     <row r="21" spans="1:64" ht="21" x14ac:dyDescent="0.4">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="30"/>
-      <c r="Z21" s="30"/>
-      <c r="AA21" s="30"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="30"/>
-      <c r="AD21" s="30"/>
-      <c r="AE21" s="30"/>
-      <c r="AF21" s="30"/>
-      <c r="AG21" s="30"/>
-      <c r="AH21" s="30"/>
-      <c r="AI21" s="30"/>
-      <c r="AJ21" s="30"/>
-      <c r="AK21" s="30"/>
-      <c r="AL21" s="30"/>
-      <c r="AM21" s="30"/>
-      <c r="AN21" s="30"/>
-      <c r="AO21" s="30"/>
-      <c r="AP21" s="30"/>
-      <c r="AQ21" s="30"/>
-      <c r="AR21" s="30"/>
-      <c r="AS21" s="30"/>
-      <c r="AT21" s="30"/>
-      <c r="AU21" s="30"/>
-      <c r="AV21" s="30"/>
-      <c r="AW21" s="30"/>
-      <c r="AX21" s="30"/>
-      <c r="AY21" s="30"/>
-      <c r="AZ21" s="30"/>
-      <c r="BA21" s="30"/>
-      <c r="BB21" s="30"/>
-      <c r="BC21" s="30"/>
-      <c r="BD21" s="30"/>
-      <c r="BE21" s="30"/>
-      <c r="BF21" s="30"/>
-      <c r="BG21" s="30"/>
-      <c r="BH21" s="30"/>
-      <c r="BI21" s="30"/>
-      <c r="BJ21" s="30"/>
-      <c r="BK21" s="30"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="39"/>
+      <c r="Z21" s="39"/>
+      <c r="AA21" s="39"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="39"/>
+      <c r="AD21" s="39"/>
+      <c r="AE21" s="39"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="39"/>
+      <c r="AH21" s="39"/>
+      <c r="AI21" s="39"/>
+      <c r="AJ21" s="39"/>
+      <c r="AK21" s="39"/>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="39"/>
+      <c r="AO21" s="39"/>
+      <c r="AP21" s="39"/>
+      <c r="AQ21" s="39"/>
+      <c r="AR21" s="39"/>
+      <c r="AS21" s="39"/>
+      <c r="AT21" s="39"/>
+      <c r="AU21" s="39"/>
+      <c r="AV21" s="39"/>
+      <c r="AW21" s="39"/>
+      <c r="AX21" s="39"/>
+      <c r="AY21" s="39"/>
+      <c r="AZ21" s="39"/>
+      <c r="BA21" s="39"/>
+      <c r="BB21" s="39"/>
+      <c r="BC21" s="39"/>
+      <c r="BD21" s="39"/>
+      <c r="BE21" s="39"/>
+      <c r="BF21" s="39"/>
+      <c r="BG21" s="39"/>
+      <c r="BH21" s="39"/>
+      <c r="BI21" s="39"/>
+      <c r="BJ21" s="39"/>
+      <c r="BK21" s="39"/>
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="28"/>
-      <c r="AH22" s="28"/>
-      <c r="AI22" s="28"/>
-      <c r="AJ22" s="28"/>
-      <c r="AK22" s="28"/>
-      <c r="AL22" s="28"/>
-      <c r="AM22" s="28"/>
-      <c r="AN22" s="28"/>
-      <c r="AO22" s="28"/>
-      <c r="AP22" s="28"/>
-      <c r="AQ22" s="28"/>
-      <c r="AR22" s="28"/>
-      <c r="AS22" s="28"/>
-      <c r="AT22" s="28"/>
-      <c r="AU22" s="28"/>
-      <c r="AV22" s="28"/>
-      <c r="AW22" s="28"/>
-      <c r="AX22" s="28"/>
-      <c r="AY22" s="28"/>
-      <c r="AZ22" s="28"/>
-      <c r="BA22" s="28"/>
-      <c r="BB22" s="28"/>
-      <c r="BC22" s="28"/>
-      <c r="BD22" s="28"/>
-      <c r="BE22" s="28"/>
-      <c r="BF22" s="28"/>
-      <c r="BG22" s="28"/>
-      <c r="BH22" s="28"/>
-      <c r="BI22" s="28"/>
-      <c r="BJ22" s="28"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="37"/>
+      <c r="Z22" s="37"/>
+      <c r="AA22" s="37"/>
+      <c r="AB22" s="37"/>
+      <c r="AC22" s="37"/>
+      <c r="AD22" s="37"/>
+      <c r="AE22" s="37"/>
+      <c r="AF22" s="37"/>
+      <c r="AG22" s="37"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="37"/>
+      <c r="AJ22" s="37"/>
+      <c r="AK22" s="37"/>
+      <c r="AL22" s="37"/>
+      <c r="AM22" s="37"/>
+      <c r="AN22" s="37"/>
+      <c r="AO22" s="37"/>
+      <c r="AP22" s="37"/>
+      <c r="AQ22" s="37"/>
+      <c r="AR22" s="37"/>
+      <c r="AS22" s="37"/>
+      <c r="AT22" s="37"/>
+      <c r="AU22" s="37"/>
+      <c r="AV22" s="37"/>
+      <c r="AW22" s="37"/>
+      <c r="AX22" s="37"/>
+      <c r="AY22" s="37"/>
+      <c r="AZ22" s="37"/>
+      <c r="BA22" s="37"/>
+      <c r="BB22" s="37"/>
+      <c r="BC22" s="37"/>
+      <c r="BD22" s="37"/>
+      <c r="BE22" s="37"/>
+      <c r="BF22" s="37"/>
+      <c r="BG22" s="37"/>
+      <c r="BH22" s="37"/>
+      <c r="BI22" s="37"/>
+      <c r="BJ22" s="37"/>
     </row>
     <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
@@ -15569,7 +15566,7 @@
       </c>
     </row>
     <row r="24" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B24">
@@ -15640,12 +15637,12 @@
       <c r="BK24">
         <v>2</v>
       </c>
-      <c r="BL24" s="29" t="s">
+      <c r="BL24" s="38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
+      <c r="A25" s="38"/>
       <c r="B25">
         <v>4</v>
       </c>
@@ -15720,10 +15717,10 @@
       <c r="BK25">
         <v>8</v>
       </c>
-      <c r="BL25" s="29"/>
+      <c r="BL25" s="38"/>
     </row>
     <row r="26" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A26" s="29"/>
+      <c r="A26" s="38"/>
       <c r="B26">
         <v>5</v>
       </c>
@@ -15810,10 +15807,10 @@
       <c r="BK26">
         <v>38</v>
       </c>
-      <c r="BL26" s="29"/>
+      <c r="BL26" s="38"/>
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
+      <c r="A27" s="38"/>
       <c r="B27">
         <v>6</v>
       </c>
@@ -15894,10 +15891,10 @@
       <c r="BK27">
         <v>10</v>
       </c>
-      <c r="BL27" s="29"/>
+      <c r="BL27" s="38"/>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
+      <c r="A28" s="38"/>
       <c r="B28">
         <v>7</v>
       </c>
@@ -15974,10 +15971,10 @@
       <c r="BK28">
         <v>7</v>
       </c>
-      <c r="BL28" s="29"/>
+      <c r="BL28" s="38"/>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
+      <c r="A29" s="38"/>
       <c r="B29">
         <v>8</v>
       </c>
@@ -16048,10 +16045,10 @@
       <c r="BK29">
         <v>2</v>
       </c>
-      <c r="BL29" s="29"/>
+      <c r="BL29" s="38"/>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A30" s="29"/>
+      <c r="A30" s="38"/>
       <c r="B30">
         <v>9</v>
       </c>
@@ -16122,10 +16119,10 @@
       <c r="BK30">
         <v>3</v>
       </c>
-      <c r="BL30" s="29"/>
+      <c r="BL30" s="38"/>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A31" s="29"/>
+      <c r="A31" s="38"/>
       <c r="B31">
         <v>10</v>
       </c>
@@ -16192,10 +16189,10 @@
       <c r="BK31">
         <v>0</v>
       </c>
-      <c r="BL31" s="29"/>
+      <c r="BL31" s="38"/>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A32" s="29"/>
+      <c r="A32" s="38"/>
       <c r="B32">
         <v>11</v>
       </c>
@@ -16262,10 +16259,10 @@
       <c r="BK32">
         <v>0</v>
       </c>
-      <c r="BL32" s="29"/>
+      <c r="BL32" s="38"/>
     </row>
     <row r="33" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A33" s="29"/>
+      <c r="A33" s="38"/>
       <c r="B33">
         <v>12</v>
       </c>
@@ -16332,10 +16329,10 @@
       <c r="BK33">
         <v>0</v>
       </c>
-      <c r="BL33" s="29"/>
+      <c r="BL33" s="38"/>
     </row>
     <row r="34" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A34" s="29"/>
+      <c r="A34" s="38"/>
       <c r="B34">
         <v>13</v>
       </c>
@@ -16402,10 +16399,10 @@
       <c r="BK34">
         <v>0</v>
       </c>
-      <c r="BL34" s="29"/>
+      <c r="BL34" s="38"/>
     </row>
     <row r="35" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A35" s="29"/>
+      <c r="A35" s="38"/>
       <c r="B35">
         <v>14</v>
       </c>
@@ -16472,10 +16469,10 @@
       <c r="BK35">
         <v>0</v>
       </c>
-      <c r="BL35" s="29"/>
+      <c r="BL35" s="38"/>
     </row>
     <row r="36" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A36" s="29"/>
+      <c r="A36" s="38"/>
       <c r="B36">
         <v>15</v>
       </c>
@@ -16542,10 +16539,10 @@
       <c r="BK36">
         <v>0</v>
       </c>
-      <c r="BL36" s="29"/>
+      <c r="BL36" s="38"/>
     </row>
     <row r="37" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A37" s="29"/>
+      <c r="A37" s="38"/>
       <c r="B37">
         <v>16</v>
       </c>
@@ -16612,10 +16609,10 @@
       <c r="BK37">
         <v>0</v>
       </c>
-      <c r="BL37" s="29"/>
+      <c r="BL37" s="38"/>
     </row>
     <row r="38" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A38" s="29"/>
+      <c r="A38" s="38"/>
       <c r="B38">
         <v>17</v>
       </c>
@@ -16682,7 +16679,7 @@
       <c r="BK38">
         <v>0</v>
       </c>
-      <c r="BL38" s="29"/>
+      <c r="BL38" s="38"/>
     </row>
     <row r="39" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B39" t="s">

</xml_diff>

<commit_message>
colors psas based on erc and fm
</commit_message>
<xml_diff>
--- a/data/DL_matrices_ID_WY.xlsx
+++ b/data/DL_matrices_ID_WY.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="GB01" sheetId="1" r:id="rId1"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BF42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BF27" sqref="BF27:BF42"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4097,8 +4097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AN32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AT27" sqref="AT27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9274,8 +9274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="BO11" sqref="BO11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BJ7" sqref="BJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9283,7 +9283,7 @@
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="2" max="2" width="3.33203125" customWidth="1"/>
     <col min="3" max="61" width="3" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="3.21875" customWidth="1"/>
+    <col min="62" max="62" width="4.88671875" customWidth="1"/>
     <col min="63" max="63" width="4.77734375" customWidth="1"/>
     <col min="64" max="64" width="3.109375" customWidth="1"/>
   </cols>
@@ -13083,8 +13083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="BN22" sqref="BN22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BJ7" sqref="BJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16889,8 +16889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BC20" sqref="BC20"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AP7" sqref="AP7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19900,8 +19900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BJ39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="BL29" sqref="BL29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BI7" sqref="BI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23503,8 +23503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BE39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BD7" sqref="BD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24226,7 +24226,7 @@
       </c>
       <c r="AR9" s="25"/>
       <c r="AS9" s="25">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AT9" s="6"/>
       <c r="AU9" s="6"/>
@@ -26569,8 +26569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BG42"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BI9" sqref="BI9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AU7" sqref="AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30201,8 +30201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BA36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG46" sqref="AG46"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AY25" sqref="AY25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>